<commit_message>
commit done by asian guy
</commit_message>
<xml_diff>
--- a/PythonDemo.xlsx
+++ b/PythonDemo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sathish Mohanraj\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sathish Mohanraj\Gitx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F2BA1D-B30C-449E-BD55-071C3C58958E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D95927-BD3F-432B-BF6A-2A5478859008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BF9CE529-8D50-4914-9811-3A45914078B1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Testcase1</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>t7</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -460,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BAFB5EA-70A6-44F5-8858-298F59D59767}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,6 +572,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
commit done by american guy
</commit_message>
<xml_diff>
--- a/PythonDemo.xlsx
+++ b/PythonDemo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sathish Mohanraj\Gitx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D95927-BD3F-432B-BF6A-2A5478859008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F742E52C-E7A6-4C11-A31A-E7E7E3BC818C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BF9CE529-8D50-4914-9811-3A45914078B1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Testcase1</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>t9</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -466,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BAFB5EA-70A6-44F5-8858-298F59D59767}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -586,6 +601,34 @@
         <v>26</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>